<commit_message>
update sha256 for passwords
</commit_message>
<xml_diff>
--- a/DataBased/UsersDB.xlsx
+++ b/DataBased/UsersDB.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\FeatherFriend\DataBased\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE00F462-DBE6-47B4-A422-7375333CB9A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A07D0AF9-D367-4566-B981-5827EECF566D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="135" yWindow="9990" windowWidth="30255" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,14 +25,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="12">
   <si>
     <t>yossiyo</t>
   </si>
   <si>
-    <t>123123WW!</t>
-  </si>
-  <si>
     <t>Username</t>
   </si>
   <si>
@@ -42,15 +39,9 @@
     <t>ID</t>
   </si>
   <si>
-    <t>Reuts1122!</t>
-  </si>
-  <si>
     <t>206452856</t>
   </si>
   <si>
-    <t>tchrz123@</t>
-  </si>
-  <si>
     <t>318692993</t>
   </si>
   <si>
@@ -63,16 +54,13 @@
     <t>omero</t>
   </si>
   <si>
-    <t>Yosi8888!</t>
-  </si>
-  <si>
-    <t>yossiso1</t>
-  </si>
-  <si>
-    <t>Tomer12!</t>
-  </si>
-  <si>
-    <t>207338351</t>
+    <t>055ef921716dabc901c32a25c6b158db41087db41d7c997aa713b4777dedcc65</t>
+  </si>
+  <si>
+    <t>reutisa</t>
+  </si>
+  <si>
+    <t>207555555</t>
   </si>
 </sst>
 </file>
@@ -411,81 +399,81 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.69921875" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.5" style="2" customWidth="1"/>
-    <col min="2" max="2" width="15" style="2" customWidth="1"/>
-    <col min="3" max="3" width="14.875" style="4" customWidth="1"/>
-    <col min="4" max="16384" width="8.75" style="2"/>
+    <col min="2" max="2" width="87.59765625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="14.8984375" style="4" customWidth="1"/>
+    <col min="4" max="16384" width="8.69921875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C2" s="4">
         <v>318638566</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>9</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>1</v>
       </c>
       <c r="C3" s="4">
         <v>213152390</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="4" t="s">
         <v>11</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>